<commit_message>
Fixes to data and scripts following inspection of GC data.
</commit_message>
<xml_diff>
--- a/SuRGE_Sharepoint/data/CIN/CH4_055_Zepernick/dataSheets/surgeData055.xlsx
+++ b/SuRGE_Sharepoint/data/CIN/CH4_055_Zepernick/dataSheets/surgeData055.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa.sharepoint.com/sites/SuRGE/Shared Documents/data/CIN/CH4_055_Zepernick/dataSheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/beaulieu_jake_epa_gov/Documents/gitRepository/SuRGE/SuRGE_Sharepoint/data/CIN/CH4_055_Zepernick/dataSheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="635" documentId="8_{C6E1C80D-2253-43E5-A6E3-4895B3CD09E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CE9D1415-9C66-47D7-B95F-E7FD8FE43ADC}"/>
+  <xr:revisionPtr revIDLastSave="641" documentId="8_{C6E1C80D-2253-43E5-A6E3-4895B3CD09E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D8981B41-8AF9-4195-A07A-F6EAC6861EF3}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16320" yWindow="-4830" windowWidth="16440" windowHeight="28320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
   <definedNames>
     <definedName name="_xlnm.Database">data!$B$2:$BQ$47</definedName>
   </definedNames>
-  <calcPr calcId="191028" concurrentManualCount="4"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -669,9 +669,6 @@
     <t>SG220625</t>
   </si>
   <si>
-    <t>SG201206</t>
-  </si>
-  <si>
     <t>SG220640</t>
   </si>
   <si>
@@ -705,12 +702,6 @@
     <t>SG220635</t>
   </si>
   <si>
-    <t>SG201207</t>
-  </si>
-  <si>
-    <t>SG201201</t>
-  </si>
-  <si>
     <t>SG220646</t>
   </si>
   <si>
@@ -723,18 +714,9 @@
     <t>SG220643</t>
   </si>
   <si>
-    <t>SG201205</t>
-  </si>
-  <si>
-    <t>SG201213</t>
-  </si>
-  <si>
     <t>SG220620</t>
   </si>
   <si>
-    <t>SG201203</t>
-  </si>
-  <si>
     <t>SG220641</t>
   </si>
   <si>
@@ -790,6 +772,24 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>SG221206</t>
+  </si>
+  <si>
+    <t>SG221205</t>
+  </si>
+  <si>
+    <t>SG221201</t>
+  </si>
+  <si>
+    <t>SG221207</t>
+  </si>
+  <si>
+    <t>SG221213</t>
+  </si>
+  <si>
+    <t>SG221203</t>
   </si>
 </sst>
 </file>
@@ -1467,9 +1467,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1507,7 +1507,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1613,7 +1613,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1755,7 +1755,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1766,84 +1766,81 @@
   <dimension ref="A1:BZ18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J23" sqref="J23"/>
+      <pane xSplit="2" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.7265625" style="24" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.54296875" customWidth="1"/>
-    <col min="5" max="5" width="10.453125" customWidth="1"/>
-    <col min="6" max="6" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.453125" customWidth="1"/>
-    <col min="19" max="19" width="16.7265625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17.7265625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.81640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="9.54296875" customWidth="1"/>
+    <col min="1" max="1" width="6.77734375" style="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" customWidth="1"/>
+    <col min="6" max="6" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.44140625" customWidth="1"/>
+    <col min="19" max="20" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.5546875" customWidth="1"/>
     <col min="28" max="28" width="9" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="5.453125" customWidth="1"/>
-    <col min="30" max="30" width="4.81640625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="6.453125" customWidth="1"/>
+    <col min="29" max="29" width="5.44140625" customWidth="1"/>
+    <col min="30" max="30" width="4.77734375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="6.44140625" customWidth="1"/>
     <col min="32" max="32" width="6" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="16.26953125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="16.77734375" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="18" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="7.26953125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="44" max="45" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="7.21875" bestFit="1" customWidth="1"/>
     <col min="47" max="47" width="8" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="4.81640625" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="5.1796875" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="6.453125" customWidth="1"/>
-    <col min="52" max="52" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="4.77734375" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="6.44140625" customWidth="1"/>
+    <col min="52" max="52" width="6.21875" bestFit="1" customWidth="1"/>
     <col min="53" max="53" width="11" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="8.77734375" bestFit="1" customWidth="1"/>
     <col min="58" max="58" width="10" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="18.26953125" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="13.77734375" bestFit="1" customWidth="1"/>
     <col min="63" max="63" width="14" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="15.1796875" bestFit="1" customWidth="1"/>
-    <col min="65" max="67" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="68" max="69" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="22.26953125" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="25.453125" customWidth="1"/>
+    <col min="64" max="64" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="65" max="69" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="22.21875" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="25.44140625" customWidth="1"/>
     <col min="74" max="74" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:78" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
@@ -1935,7 +1932,7 @@
       <c r="BY1" s="31"/>
       <c r="BZ1" s="31"/>
     </row>
-    <row r="2" spans="1:78" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A2" s="23" t="s">
         <v>6</v>
       </c>
@@ -2057,7 +2054,7 @@
         <v>40</v>
       </c>
       <c r="AO2" s="7" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AP2" s="7" t="s">
         <v>41</v>
@@ -2078,7 +2075,7 @@
         <v>46</v>
       </c>
       <c r="AV2" s="7" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="AW2" s="7" t="s">
         <v>47</v>
@@ -2123,7 +2120,7 @@
         <v>59</v>
       </c>
       <c r="BK2" s="7" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="BL2" s="7" t="s">
         <v>60</v>
@@ -2144,7 +2141,7 @@
         <v>65</v>
       </c>
       <c r="BR2" s="7" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="BS2" s="7" t="s">
         <v>66</v>
@@ -2171,7 +2168,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:78" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A3" s="24" t="s">
         <v>173</v>
       </c>
@@ -2188,13 +2185,13 @@
         <v>80.980119999999999</v>
       </c>
       <c r="F3" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="G3" s="27">
         <v>0.35625000000000001</v>
       </c>
       <c r="H3" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="I3" s="27">
         <v>0.39305555555555555</v>
@@ -2206,13 +2203,13 @@
         <v>204</v>
       </c>
       <c r="N3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="P3" t="s">
-        <v>228</v>
+        <v>248</v>
       </c>
       <c r="T3" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="U3" s="28">
         <v>0.52644675925925932</v>
@@ -2278,13 +2275,13 @@
         <v>3.26</v>
       </c>
       <c r="BT3" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="BU3" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="BV3" s="28" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="BW3">
         <v>1.7501</v>
@@ -2293,13 +2290,13 @@
         <v>409.66</v>
       </c>
       <c r="BY3" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="BZ3" s="28">
         <v>0.5294444444444445</v>
       </c>
     </row>
-    <row r="4" spans="1:78" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A4" s="24" t="s">
         <v>173</v>
       </c>
@@ -2316,13 +2313,13 @@
         <v>80.980130000000003</v>
       </c>
       <c r="F4" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="G4" s="27">
         <v>0.3611111111111111</v>
       </c>
       <c r="H4" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="I4" s="27">
         <v>0.41597222222222219</v>
@@ -2331,13 +2328,13 @@
         <v>41</v>
       </c>
       <c r="L4" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="N4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="T4" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="U4" s="28">
         <v>0.36476851851851855</v>
@@ -2406,7 +2403,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="5" spans="1:78" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A5" s="24" t="s">
         <v>173</v>
       </c>
@@ -2423,13 +2420,13 @@
         <v>80.980760000000004</v>
       </c>
       <c r="F5" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="G5" s="27">
         <v>0.37222222222222223</v>
       </c>
       <c r="H5" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="I5" s="27">
         <v>0.40625</v>
@@ -2441,10 +2438,10 @@
         <v>205</v>
       </c>
       <c r="N5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="T5" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="U5" s="28">
         <v>0.37615740740740744</v>
@@ -2510,7 +2507,7 @@
         <v>11.56</v>
       </c>
     </row>
-    <row r="6" spans="1:78" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A6" s="24" t="s">
         <v>173</v>
       </c>
@@ -2527,13 +2524,13 @@
         <v>80.982299999999995</v>
       </c>
       <c r="F6" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="G6" s="27">
         <v>0.38611111111111113</v>
       </c>
       <c r="H6" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="I6" s="27">
         <v>0.41666666666666669</v>
@@ -2545,13 +2542,13 @@
         <v>206</v>
       </c>
       <c r="N6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="P6" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="T6" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="U6" s="28">
         <v>0.38842592592592595</v>
@@ -2626,7 +2623,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="7" spans="1:78" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A7" s="24" t="s">
         <v>173</v>
       </c>
@@ -2643,13 +2640,13 @@
         <v>80.980959999999996</v>
       </c>
       <c r="F7" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="G7" s="27">
         <v>0.39583333333333331</v>
       </c>
       <c r="H7" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="I7" s="27">
         <v>0.41180555555555554</v>
@@ -2661,10 +2658,10 @@
         <v>207</v>
       </c>
       <c r="N7" t="s">
-        <v>221</v>
+        <v>247</v>
       </c>
       <c r="T7" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="U7" s="28">
         <v>0.39693287037037034</v>
@@ -2739,7 +2736,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="8" spans="1:78" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A8" s="24" t="s">
         <v>173</v>
       </c>
@@ -2756,13 +2753,13 @@
         <v>80.982699999999994</v>
       </c>
       <c r="F8" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="G8" s="27">
         <v>0.41041666666666665</v>
       </c>
       <c r="H8" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="I8" s="27">
         <v>0.42708333333333331</v>
@@ -2774,10 +2771,10 @@
         <v>208</v>
       </c>
       <c r="N8" t="s">
-        <v>222</v>
+        <v>246</v>
       </c>
       <c r="T8" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="U8" s="28">
         <v>0.42456018518518518</v>
@@ -2843,7 +2840,7 @@
         <v>24.63</v>
       </c>
     </row>
-    <row r="9" spans="1:78" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A9" s="24" t="s">
         <v>173</v>
       </c>
@@ -2860,13 +2857,13 @@
         <v>80.982039999999998</v>
       </c>
       <c r="F9" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="G9" s="27">
         <v>0.43472222222222223</v>
       </c>
       <c r="H9" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="I9" s="27">
         <v>0.4694444444444445</v>
@@ -2875,10 +2872,10 @@
         <v>13</v>
       </c>
       <c r="L9" t="s">
-        <v>209</v>
+        <v>244</v>
       </c>
       <c r="T9" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="U9" s="28">
         <v>0.43535879629629631</v>
@@ -2947,7 +2944,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="10" spans="1:78" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A10" s="24" t="s">
         <v>173</v>
       </c>
@@ -2964,13 +2961,13 @@
         <v>80.982439999999997</v>
       </c>
       <c r="F10" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="G10" s="27">
         <v>0.44305555555555554</v>
       </c>
       <c r="H10" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="I10" s="27">
         <v>0.47569444444444442</v>
@@ -2979,13 +2976,13 @@
         <v>53</v>
       </c>
       <c r="L10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="N10" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="T10" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="U10" s="28">
         <v>0.44496527777777778</v>
@@ -3060,7 +3057,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="11" spans="1:78" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A11" s="24" t="s">
         <v>173</v>
       </c>
@@ -3077,13 +3074,13 @@
         <v>80.98272</v>
       </c>
       <c r="F11" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="G11" s="27">
         <v>0.45416666666666666</v>
       </c>
       <c r="H11" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="I11" s="27">
         <v>0.48333333333333334</v>
@@ -3092,10 +3089,10 @@
         <v>30</v>
       </c>
       <c r="L11" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="T11" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="U11" s="28">
         <v>0.45572916666666669</v>
@@ -3164,7 +3161,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="12" spans="1:78" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A12" s="24" t="s">
         <v>173</v>
       </c>
@@ -3181,31 +3178,31 @@
         <v>80.983000000000004</v>
       </c>
       <c r="F12" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="G12" s="27">
         <v>0.46180555555555558</v>
       </c>
       <c r="H12" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="I12" s="27">
         <v>0.4909722222222222</v>
       </c>
       <c r="J12" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="K12" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="R12">
         <v>1</v>
       </c>
       <c r="S12" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="T12" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="U12" s="28">
         <v>0.46283564814814815</v>
@@ -3274,7 +3271,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="13" spans="1:78" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
         <v>173</v>
       </c>
@@ -3291,13 +3288,13 @@
         <v>80.981859999999998</v>
       </c>
       <c r="F13" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="G13" s="27">
         <v>0.4694444444444445</v>
       </c>
       <c r="H13" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="I13" s="27">
         <v>0.49722222222222223</v>
@@ -3306,10 +3303,10 @@
         <v>23</v>
       </c>
       <c r="L13" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="T13" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="U13" s="28">
         <v>0.47188657407407408</v>
@@ -3375,7 +3372,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:78" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A14" s="24" t="s">
         <v>173</v>
       </c>
@@ -3392,13 +3389,13 @@
         <v>80.98066</v>
       </c>
       <c r="F14" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="G14" s="27">
         <v>0.47638888888888892</v>
       </c>
       <c r="H14" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="I14" s="27">
         <v>0.51180555555555551</v>
@@ -3407,16 +3404,16 @@
         <v>64</v>
       </c>
       <c r="L14" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="N14" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="P14" t="s">
-        <v>230</v>
+        <v>249</v>
       </c>
       <c r="T14" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="U14" s="28">
         <v>0.4801273148148148</v>
@@ -3482,7 +3479,7 @@
         <v>6.22</v>
       </c>
     </row>
-    <row r="15" spans="1:78" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A15" s="24" t="s">
         <v>173</v>
       </c>
@@ -3499,13 +3496,13 @@
         <v>80.979929999999996</v>
       </c>
       <c r="F15" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="G15" s="27">
         <v>0.5</v>
       </c>
       <c r="H15" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="I15" s="27">
         <v>0.50763888888888886</v>
@@ -3514,16 +3511,16 @@
         <v>85</v>
       </c>
       <c r="L15" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="N15" t="s">
+        <v>222</v>
+      </c>
+      <c r="P15" t="s">
         <v>225</v>
       </c>
-      <c r="P15" t="s">
+      <c r="T15" t="s">
         <v>231</v>
-      </c>
-      <c r="T15" t="s">
-        <v>237</v>
       </c>
       <c r="U15" s="28">
         <v>0.50069444444444444</v>
@@ -3589,7 +3586,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="16" spans="1:78" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A16" s="24" t="s">
         <v>173</v>
       </c>
@@ -3606,13 +3603,13 @@
         <v>80.981350000000006</v>
       </c>
       <c r="F16" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="G16" s="27">
         <v>0.50624999999999998</v>
       </c>
       <c r="H16" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="I16" s="27">
         <v>0.50416666666666665</v>
@@ -3621,16 +3618,16 @@
         <v>95</v>
       </c>
       <c r="L16" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="N16" t="s">
+        <v>223</v>
+      </c>
+      <c r="P16" t="s">
         <v>226</v>
       </c>
-      <c r="P16" t="s">
-        <v>232</v>
-      </c>
       <c r="T16" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="U16" s="28">
         <v>0.50752314814814814</v>
@@ -3696,7 +3693,7 @@
         <v>6.78</v>
       </c>
     </row>
-    <row r="17" spans="1:57" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A17" s="24" t="s">
         <v>173</v>
       </c>
@@ -3713,13 +3710,13 @@
         <v>80.979399999999998</v>
       </c>
       <c r="F17" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="G17" s="27">
         <v>0.51736111111111105</v>
       </c>
       <c r="H17" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="I17" s="27">
         <v>0.3979166666666667</v>
@@ -3728,13 +3725,13 @@
         <v>36</v>
       </c>
       <c r="L17" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N17" t="s">
-        <v>227</v>
+        <v>245</v>
       </c>
       <c r="T17" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="U17" s="28">
         <v>0.51909722222222221</v>
@@ -3800,7 +3797,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="18" spans="1:57" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A18" s="24" t="s">
         <v>173</v>
       </c>
@@ -3834,15 +3831,15 @@
       <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.7265625" style="26" customWidth="1"/>
-    <col min="2" max="2" width="116.7265625" style="26" customWidth="1"/>
-    <col min="3" max="3" width="49.54296875" style="26" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.1796875" style="26"/>
+    <col min="1" max="1" width="26.77734375" style="26" customWidth="1"/>
+    <col min="2" max="2" width="116.77734375" style="26" customWidth="1"/>
+    <col min="3" max="3" width="49.5546875" style="26" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.21875" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>74</v>
       </c>
@@ -3853,7 +3850,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -3864,7 +3861,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -3875,7 +3872,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>8</v>
       </c>
@@ -3886,7 +3883,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -3897,7 +3894,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -3908,7 +3905,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -3919,7 +3916,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -3930,7 +3927,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -3941,7 +3938,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -3952,7 +3949,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -3963,7 +3960,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -3974,7 +3971,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -3985,7 +3982,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -3994,7 +3991,7 @@
       </c>
       <c r="C14"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -4005,7 +4002,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -4014,7 +4011,7 @@
       </c>
       <c r="C16"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -4025,7 +4022,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -4034,7 +4031,7 @@
       </c>
       <c r="C18"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>101</v>
       </c>
@@ -4045,7 +4042,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>104</v>
       </c>
@@ -4054,7 +4051,7 @@
       </c>
       <c r="C20"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -4065,7 +4062,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -4076,7 +4073,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -4087,7 +4084,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -4098,7 +4095,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -4109,7 +4106,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>112</v>
       </c>
@@ -4120,7 +4117,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>113</v>
       </c>
@@ -4129,7 +4126,7 @@
       </c>
       <c r="C27"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -4140,7 +4137,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -4151,7 +4148,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -4162,7 +4159,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -4173,7 +4170,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -4184,7 +4181,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -4195,7 +4192,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -4206,18 +4203,18 @@
         <v>124</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>192</v>
       </c>
       <c r="B35" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="C35" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -4228,7 +4225,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -4237,7 +4234,7 @@
       </c>
       <c r="C37"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -4246,7 +4243,7 @@
       </c>
       <c r="C38"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -4255,7 +4252,7 @@
       </c>
       <c r="C39"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -4264,7 +4261,7 @@
       </c>
       <c r="C40"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -4273,16 +4270,16 @@
       </c>
       <c r="C41"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="B42" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="C42"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -4291,7 +4288,7 @@
       </c>
       <c r="C43"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -4300,7 +4297,7 @@
       </c>
       <c r="C44"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -4309,7 +4306,7 @@
       </c>
       <c r="C45"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>44</v>
       </c>
@@ -4318,7 +4315,7 @@
       </c>
       <c r="C46"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>45</v>
       </c>
@@ -4327,7 +4324,7 @@
       </c>
       <c r="C47"/>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -4336,16 +4333,16 @@
       </c>
       <c r="C48"/>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="B49" t="s">
         <v>133</v>
       </c>
       <c r="C49"/>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>47</v>
       </c>
@@ -4354,7 +4351,7 @@
       </c>
       <c r="C50"/>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>48</v>
       </c>
@@ -4365,7 +4362,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>49</v>
       </c>
@@ -4376,7 +4373,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>50</v>
       </c>
@@ -4387,7 +4384,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>51</v>
       </c>
@@ -4398,7 +4395,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>52</v>
       </c>
@@ -4409,7 +4406,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>53</v>
       </c>
@@ -4420,18 +4417,18 @@
         <v>124</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>195</v>
       </c>
       <c r="B57" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="C57" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>54</v>
       </c>
@@ -4442,7 +4439,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>55</v>
       </c>
@@ -4451,7 +4448,7 @@
       </c>
       <c r="C59"/>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>56</v>
       </c>
@@ -4460,7 +4457,7 @@
       </c>
       <c r="C60"/>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>57</v>
       </c>
@@ -4469,7 +4466,7 @@
       </c>
       <c r="C61"/>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>58</v>
       </c>
@@ -4478,7 +4475,7 @@
       </c>
       <c r="C62"/>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>59</v>
       </c>
@@ -4487,16 +4484,16 @@
       </c>
       <c r="C63"/>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="B64" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="C64"/>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>60</v>
       </c>
@@ -4505,7 +4502,7 @@
       </c>
       <c r="C65"/>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>61</v>
       </c>
@@ -4514,7 +4511,7 @@
       </c>
       <c r="C66"/>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>62</v>
       </c>
@@ -4523,7 +4520,7 @@
       </c>
       <c r="C67"/>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>63</v>
       </c>
@@ -4532,7 +4529,7 @@
       </c>
       <c r="C68"/>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>64</v>
       </c>
@@ -4541,7 +4538,7 @@
       </c>
       <c r="C69"/>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>65</v>
       </c>
@@ -4550,16 +4547,16 @@
       </c>
       <c r="C70"/>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="B71" t="s">
         <v>133</v>
       </c>
       <c r="C71"/>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>66</v>
       </c>
@@ -4568,7 +4565,7 @@
       </c>
       <c r="C72"/>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>67</v>
       </c>
@@ -4579,7 +4576,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>68</v>
       </c>
@@ -4590,7 +4587,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>69</v>
       </c>
@@ -4601,7 +4598,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>70</v>
       </c>
@@ -4612,7 +4609,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>71</v>
       </c>
@@ -4623,7 +4620,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>72</v>
       </c>
@@ -4634,7 +4631,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>73</v>
       </c>
@@ -4645,7 +4642,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80"/>
       <c r="B80"/>
       <c r="C80"/>
@@ -4663,17 +4660,17 @@
       <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.81640625" style="24"/>
-    <col min="3" max="3" width="15.453125" customWidth="1"/>
-    <col min="5" max="5" width="13.26953125" customWidth="1"/>
-    <col min="7" max="7" width="12.26953125" customWidth="1"/>
-    <col min="9" max="9" width="14.26953125" customWidth="1"/>
+    <col min="1" max="1" width="8.77734375" style="24"/>
+    <col min="3" max="3" width="15.44140625" customWidth="1"/>
+    <col min="5" max="5" width="13.21875" customWidth="1"/>
+    <col min="7" max="7" width="12.21875" customWidth="1"/>
+    <col min="9" max="9" width="14.21875" customWidth="1"/>
     <col min="10" max="10" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="37" t="s">
         <v>5</v>
       </c>
@@ -4689,7 +4686,7 @@
       <c r="K1" s="19"/>
       <c r="L1" s="19"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -4723,7 +4720,7 @@
       <c r="K2" s="3"/>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="24" t="s">
         <v>173</v>
       </c>
@@ -4752,7 +4749,7 @@
         <v>28.9</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="24" t="s">
         <v>173</v>
       </c>
@@ -4781,7 +4778,7 @@
         <v>28.9</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="24" t="s">
         <v>173</v>
       </c>
@@ -4810,7 +4807,7 @@
         <v>28.9</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="24" t="s">
         <v>173</v>
       </c>
@@ -4839,7 +4836,7 @@
         <v>28.9</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="24" t="s">
         <v>173</v>
       </c>
@@ -4868,7 +4865,7 @@
         <v>28.9</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="24" t="s">
         <v>173</v>
       </c>
@@ -4915,14 +4912,14 @@
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="63.54296875" customWidth="1"/>
-    <col min="3" max="3" width="49.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.5546875" customWidth="1"/>
+    <col min="3" max="3" width="49.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>74</v>
       </c>
@@ -4933,7 +4930,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -4944,7 +4941,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -4955,7 +4952,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
         <v>154</v>
       </c>
@@ -4966,7 +4963,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>155</v>
       </c>
@@ -4977,7 +4974,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
         <v>156</v>
       </c>
@@ -4988,7 +4985,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="21" t="s">
         <v>157</v>
       </c>
@@ -4996,7 +4993,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
         <v>158</v>
       </c>
@@ -5007,7 +5004,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
         <v>159</v>
       </c>
@@ -5018,7 +5015,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="22" t="s">
         <v>160</v>
       </c>
@@ -5029,7 +5026,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
         <v>161</v>
       </c>
@@ -5046,11 +5043,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="29f62856-1543-49d4-a736-4569d363f533" ContentTypeId="0x0101" PreviousValue="false"/>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -5059,49 +5051,12 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Record xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">Shared</Record>
-    <Language xmlns="http://schemas.microsoft.com/sharepoint/v3">English</Language>
-    <Document_x0020_Creation_x0020_Date xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">2020-10-21T13:32:44+00:00</Document_x0020_Creation_x0020_Date>
-    <_Source xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-    <j747ac98061d40f0aa7bd47e1db5675d xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </j747ac98061d40f0aa7bd47e1db5675d>
-    <External_x0020_Contributor xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <TaxKeywordTaxHTField xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-    <Rights xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <EPA_x0020_Office xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <CategoryDescription xmlns="http://schemas.microsoft.com/sharepoint.v3" xsi:nil="true"/>
-    <Identifier xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <_Coverage xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-    <Creator xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Creator>
-    <EPA_x0020_Related_x0020_Documents xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <EPA_x0020_Contributor xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </EPA_x0020_Contributor>
-    <TaxCatchAll xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ed970698-2d60-4bab-a048-d9be527522d9">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="29f62856-1543-49d4-a736-4569d363f533" ContentTypeId="0x0101" PreviousValue="false"/>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001AF5FC5DD832BE4DBA6B24560DD3ADC0" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d40b3e6283001fb57e5088f84fb23d5e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xmlns:ns3="http://schemas.microsoft.com/sharepoint.v3" xmlns:ns4="http://schemas.microsoft.com/sharepoint/v3/fields" xmlns:ns5="8b03727f-4454-4722-b3e6-018d8dcaf2fd" xmlns:ns6="ed970698-2d60-4bab-a048-d9be527522d9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="aadbb8160917885bdc8cfb32badaafe9" ns1:_="" ns2:_="" ns3:_="" ns4:_="" ns5:_="" ns6:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -5572,7 +5527,57 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Record xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">Shared</Record>
+    <Language xmlns="http://schemas.microsoft.com/sharepoint/v3">English</Language>
+    <Document_x0020_Creation_x0020_Date xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">2020-10-21T13:32:44+00:00</Document_x0020_Creation_x0020_Date>
+    <_Source xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+    <j747ac98061d40f0aa7bd47e1db5675d xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </j747ac98061d40f0aa7bd47e1db5675d>
+    <External_x0020_Contributor xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <TaxKeywordTaxHTField xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+    <Rights xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <EPA_x0020_Office xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <CategoryDescription xmlns="http://schemas.microsoft.com/sharepoint.v3" xsi:nil="true"/>
+    <Identifier xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <_Coverage xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+    <Creator xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Creator>
+    <EPA_x0020_Related_x0020_Documents xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <EPA_x0020_Contributor xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </EPA_x0020_Contributor>
+    <TaxCatchAll xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ed970698-2d60-4bab-a048-d9be527522d9">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F4A5FCF-4499-487A-89B0-E215184C11DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{845EA28A-135D-4CD8-9991-40FEAFECD172}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
@@ -5580,29 +5585,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F4A5FCF-4499-487A-89B0-E215184C11DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D26D44A-9508-4707-B138-18882E5BA6FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
-    <ds:schemaRef ds:uri="ed970698-2d60-4bab-a048-d9be527522d9"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{55DAE491-7D98-45ED-B924-7B028C910407}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5623,4 +5606,18 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D26D44A-9508-4707-B138-18882E5BA6FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
+    <ds:schemaRef ds:uri="ed970698-2d60-4bab-a048-d9be527522d9"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>